<commit_message>
break-down các task cho màn hình handheld
</commit_message>
<xml_diff>
--- a/documents/outsources/Tasks-print2.xlsx
+++ b/documents/outsources/Tasks-print2.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="outsource" sheetId="1" r:id="rId1"/>
+    <sheet name="Handheld" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">E30; E20; E33; E80 </t>
   </si>
@@ -97,6 +98,27 @@
   </si>
   <si>
     <t>POST api/v2/sites/{siteId}/global-item-searchs</t>
+  </si>
+  <si>
+    <t>GET api/v2/{siteId}/che/{cheId}/workinstructions</t>
+  </si>
+  <si>
+    <t>GET api/v2/{siteId}/req-wis</t>
+  </si>
+  <si>
+    <t>GET api/v2/{siteId}/res-wis/{fromDate}/{toDate}</t>
+  </si>
+  <si>
+    <t>GET api/v2/{siteId}/done-wis/{fromDate}/{toDate}</t>
+  </si>
+  <si>
+    <t>GET api/v2/{siteId}/del-req-wis</t>
+  </si>
+  <si>
+    <t>GET api/v2/{siteId}/del-res-wis/{fromData}/{toDate}</t>
+  </si>
+  <si>
+    <t>PUT api/v2/{siteId}/che/{cheId}/wis/{wiid}</t>
   </si>
 </sst>
 </file>
@@ -104,7 +126,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -137,10 +159,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -437,7 +459,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -460,7 +482,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="2"/>
       <c r="B2">
         <v>1</v>
       </c>
@@ -478,13 +500,13 @@
         <f>E2/60</f>
         <v>34</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <f>F2*80000</f>
         <v>2720000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2"/>
       <c r="B3">
         <v>2</v>
       </c>
@@ -496,7 +518,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4">
         <v>3</v>
       </c>
@@ -508,7 +530,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5">
         <v>4</v>
       </c>
@@ -520,7 +542,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
       <c r="B6">
         <v>5</v>
       </c>
@@ -532,7 +554,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2"/>
       <c r="B7">
         <v>6</v>
       </c>
@@ -544,7 +566,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2"/>
       <c r="B8">
         <v>7</v>
       </c>
@@ -556,7 +578,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
       <c r="B9">
         <v>8</v>
       </c>
@@ -568,7 +590,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
       <c r="B10">
         <v>9</v>
       </c>
@@ -580,7 +602,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11">
         <v>10</v>
       </c>
@@ -592,7 +614,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
       <c r="B12">
         <v>11</v>
       </c>
@@ -604,7 +626,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="2"/>
       <c r="B13">
         <v>12</v>
       </c>
@@ -616,7 +638,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B14">
@@ -630,7 +652,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2"/>
       <c r="B15">
         <v>14</v>
       </c>
@@ -642,7 +664,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16">
@@ -656,7 +678,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="2"/>
       <c r="B17">
         <v>16</v>
       </c>
@@ -668,7 +690,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
       <c r="B18">
         <v>17</v>
       </c>
@@ -688,4 +710,58 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="85.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>